<commit_message>
Trung Fix Kiểm Thử sprint 1 bản 1.1
</commit_message>
<xml_diff>
--- a/Sprint 1/Tài liệu đặc tả yêu cầu/KIểm Thử ONLY QUẠT test.xlsx
+++ b/Sprint 1/Tài liệu đặc tả yêu cầu/KIểm Thử ONLY QUẠT test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\BCS\Sprint 1\Tài liệu đặc tả yêu cầu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D12545B-C246-4C87-AFA5-EC87A1686DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B484D816-A732-43F9-A842-285917F68D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43FC9F9E-2304-46AE-ABF6-86A58265D84E}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="172">
   <si>
     <t>Test case: Trang chủ BCS</t>
   </si>
@@ -622,6 +622,9 @@
   </si>
   <si>
     <t>D_32</t>
+  </si>
+  <si>
+    <t>Trang đăng nhập</t>
   </si>
 </sst>
 </file>
@@ -926,7 +929,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1010,6 +1013,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1052,32 +1061,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1395,8 +1383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AD530AB-72E8-4A06-B006-BA90A153AC6B}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1411,32 +1399,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="29" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1471,7 +1459,7 @@
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="34" t="s">
         <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1497,10 +1485,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="32"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="10" t="s">
         <v>17</v>
       </c>
@@ -1524,10 +1512,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="32"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="10" t="s">
         <v>32</v>
       </c>
@@ -1551,10 +1539,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="32"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="9" t="s">
         <v>20</v>
       </c>
@@ -1578,10 +1566,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="32"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="9" t="s">
         <v>23</v>
       </c>
@@ -1605,10 +1593,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="32"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="9" t="s">
         <v>26</v>
       </c>
@@ -1632,10 +1620,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="32"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="9" t="s">
         <v>29</v>
       </c>
@@ -1669,32 +1657,32 @@
       <c r="I11" s="19"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="29" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
@@ -1729,7 +1717,7 @@
       <c r="A16" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="35" t="s">
         <v>54</v>
       </c>
       <c r="C16" s="7" t="s">
@@ -1752,7 +1740,7 @@
       <c r="A17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="33"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="9" t="s">
         <v>43</v>
       </c>
@@ -1779,7 +1767,7 @@
       <c r="A18" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="33"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="9" t="s">
         <v>43</v>
       </c>
@@ -1806,7 +1794,7 @@
       <c r="A19" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B19" s="33"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="9" t="s">
         <v>48</v>
       </c>
@@ -1833,7 +1821,7 @@
       <c r="A20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="33"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="9" t="s">
         <v>50</v>
       </c>
@@ -1867,32 +1855,32 @@
       <c r="I21" s="19"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="29" t="s">
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
     </row>
     <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
@@ -1927,6 +1915,9 @@
       <c r="A26" s="5" t="s">
         <v>75</v>
       </c>
+      <c r="B26" s="35" t="s">
+        <v>171</v>
+      </c>
       <c r="C26" s="7" t="s">
         <v>12</v>
       </c>
@@ -1953,6 +1944,7 @@
       <c r="A27" s="5" t="s">
         <v>76</v>
       </c>
+      <c r="B27" s="35"/>
       <c r="C27" s="9" t="s">
         <v>43</v>
       </c>
@@ -1979,6 +1971,7 @@
       <c r="A28" s="5" t="s">
         <v>77</v>
       </c>
+      <c r="B28" s="35"/>
       <c r="C28" s="9" t="s">
         <v>63</v>
       </c>
@@ -2005,6 +1998,7 @@
       <c r="A29" s="5" t="s">
         <v>78</v>
       </c>
+      <c r="B29" s="35"/>
       <c r="C29" s="9" t="s">
         <v>65</v>
       </c>
@@ -2031,6 +2025,7 @@
       <c r="A30" s="5" t="s">
         <v>79</v>
       </c>
+      <c r="B30" s="35"/>
       <c r="C30" s="9" t="s">
         <v>65</v>
       </c>
@@ -2057,6 +2052,7 @@
       <c r="A31" s="5" t="s">
         <v>80</v>
       </c>
+      <c r="B31" s="35"/>
       <c r="C31" s="9" t="s">
         <v>69</v>
       </c>
@@ -2083,6 +2079,7 @@
       <c r="A32" s="5" t="s">
         <v>81</v>
       </c>
+      <c r="B32" s="35"/>
       <c r="C32" s="9" t="s">
         <v>65</v>
       </c>
@@ -2106,19 +2103,19 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="29" t="s">
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="14" t="s">
@@ -2166,7 +2163,7 @@
       <c r="A38" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="30" t="s">
         <v>87</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -2195,7 +2192,7 @@
       <c r="A39" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B39" s="46"/>
+      <c r="B39" s="30"/>
       <c r="C39" s="5" t="s">
         <v>88</v>
       </c>
@@ -2222,7 +2219,7 @@
       <c r="A40" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B40" s="46"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="5" t="s">
         <v>95</v>
       </c>
@@ -2246,34 +2243,34 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="49" t="s">
+      <c r="A41" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B41" s="46"/>
-      <c r="C41" s="47" t="s">
+      <c r="B41" s="30"/>
+      <c r="C41" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="D41" s="51" t="s">
+      <c r="D41" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="E41" s="48" t="s">
+      <c r="E41" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="F41" s="49" t="s">
+      <c r="F41" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="G41" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="I41" s="50" t="s">
+      <c r="G41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="10" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
     <mergeCell ref="B38:B41"/>
     <mergeCell ref="G35:I35"/>
     <mergeCell ref="A35:F35"/>
@@ -2288,6 +2285,7 @@
     <mergeCell ref="A14:I14"/>
     <mergeCell ref="B16:B20"/>
     <mergeCell ref="G23:I23"/>
+    <mergeCell ref="B26:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2313,11 +2311,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="36"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
       <c r="D1" s="20"/>
       <c r="E1" s="20"/>
       <c r="F1" s="20"/>
@@ -2327,18 +2325,18 @@
       <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="39"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
@@ -2376,7 +2374,7 @@
       <c r="A4" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="42" t="s">
         <v>125</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -2404,7 +2402,7 @@
       <c r="A5" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="41"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="9" t="s">
         <v>111</v>
       </c>
@@ -2430,7 +2428,7 @@
       <c r="A6" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="41"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="9" t="s">
         <v>113</v>
       </c>
@@ -2456,7 +2454,7 @@
       <c r="A7" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B7" s="41"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="9" t="s">
         <v>116</v>
       </c>
@@ -2482,7 +2480,7 @@
       <c r="A8" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B8" s="42"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="9" t="s">
         <v>118</v>
       </c>
@@ -2506,11 +2504,11 @@
     </row>
     <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
@@ -2520,18 +2518,18 @@
       <c r="J11" s="21"/>
     </row>
     <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="41"/>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
@@ -2569,7 +2567,7 @@
       <c r="A14" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="42" t="s">
         <v>127</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -2597,7 +2595,7 @@
       <c r="A15" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B15" s="41"/>
+      <c r="B15" s="43"/>
       <c r="C15" s="9" t="s">
         <v>129</v>
       </c>
@@ -2623,7 +2621,7 @@
       <c r="A16" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B16" s="41"/>
+      <c r="B16" s="43"/>
       <c r="C16" s="9" t="s">
         <v>130</v>
       </c>
@@ -2649,7 +2647,7 @@
       <c r="A17" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B17" s="41"/>
+      <c r="B17" s="43"/>
       <c r="C17" s="9" t="s">
         <v>131</v>
       </c>
@@ -2675,7 +2673,7 @@
       <c r="A18" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B18" s="42"/>
+      <c r="B18" s="44"/>
       <c r="C18" s="9" t="s">
         <v>132</v>
       </c>
@@ -2699,11 +2697,11 @@
     </row>
     <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="36"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="38"/>
       <c r="D21" s="20"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
@@ -2713,18 +2711,18 @@
       <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="38"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="39"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="41"/>
     </row>
     <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
@@ -2762,7 +2760,7 @@
       <c r="A24" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="45" t="s">
         <v>166</v>
       </c>
       <c r="C24" s="20" t="s">
@@ -2790,7 +2788,7 @@
       <c r="A25" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B25" s="45"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="20" t="s">
         <v>150</v>
       </c>
@@ -2841,21 +2839,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Tài liệu" ma:contentTypeID="0x0101005FB192C60D8CDA479E1E05FDE69506A9" ma:contentTypeVersion="4" ma:contentTypeDescription="Tạo tài liệu mới." ma:contentTypeScope="" ma:versionID="86e0b5d8f6cd43469d4b0198d476de1e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1e5bcc28-56d4-4657-8a9b-4429cf64ad81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddbbbd0f9bf0d1f20f4eb87448aec86e" ns3:_="">
     <xsd:import namespace="1e5bcc28-56d4-4657-8a9b-4429cf64ad81"/>
@@ -2999,10 +2982,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA0D93D3-DA8A-4B83-9EDB-2F2D1B43D768}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABAC459C-3283-4A1D-9A28-344C07F57AE0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e5bcc28-56d4-4657-8a9b-4429cf64ad81"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3024,19 +3032,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABAC459C-3283-4A1D-9A28-344C07F57AE0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA0D93D3-DA8A-4B83-9EDB-2F2D1B43D768}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e5bcc28-56d4-4657-8a9b-4429cf64ad81"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>